<commit_message>
Minimum Requirements Definitions - added as individual guide and into tool
</commit_message>
<xml_diff>
--- a/Data Collection Tools/01 - Site Lead - Minimum Requirements Formatted Checklist_04082019.xlsx
+++ b/Data Collection Tools/01 - Site Lead - Minimum Requirements Formatted Checklist_04082019.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vka5\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\10-10 Documents\Siyenza\Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11850" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Facility List" sheetId="2" r:id="rId2"/>
+    <sheet name="Definitions" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="207">
   <si>
     <t>Minimum Requirements</t>
   </si>
@@ -583,13 +584,120 @@
   </si>
   <si>
     <t>2.4 Has the facility had sufficient TPT stocks consistently for the last 3 months?</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Definition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This indicator is looking for ID that are unique to SA as a whole, not the facility level (i.e. HPRS). </t>
+  </si>
+  <si>
+    <t>This indicator is looking to identify if screening is integrated at the first point of patient contact. Triage is central and all patients must pass through this. If no triage exists, screening of all patients should occur at the point where vital signs are taken.</t>
+  </si>
+  <si>
+    <t>This refers to patient outcomes at the final point, i.e. whether or not they returned to the facility after tracking/tracing (i.e. confirmed in Tier.net).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is to clarify if the providers have access to patient results online from within the facility.  </t>
+  </si>
+  <si>
+    <t>Is there a system in place to allow return patients that have been non-adherent to access care directly and bypass a long wait?</t>
+  </si>
+  <si>
+    <t>This indicator refers to stationary provided by the NDOH. Partners may provide stationary, but this is to specifically track provision by NDOH.</t>
+  </si>
+  <si>
+    <t>2.2 Does the facility dispense 3 months of ART for all stable patients on ART for longer than 6 months?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Some clinics, especially in the Gauteng province, may be providing a 2 month supply. Even if this is standard for the facility and the policy for the region, this would still be answered as a “NO”.  We are negotiating with NDOH to provide 3-month prescriptions in the near future. </t>
+  </si>
+  <si>
+    <r>
+      <t>Please query if they have available 1</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>st</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> line and 2</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> line ARVs including adult and pediatric formulations (please reference annex with formulations – 2016 ARV guidelines before July/2019 ARV guidelines from August).</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">This indicator refers to stock supplied by national systems.  If partners are procuring, please list this as a no.  </t>
+  </si>
+  <si>
+    <t>Is there a specific private space where HIV testing services can be provided in each sector (i.e. Acute, chronic, MCH, and ideally accident/emergency)?</t>
+  </si>
+  <si>
+    <t>This indicator looks both at space in the facility for capturing data and connectivity. If either connectivity or space is inadequate, answer as “NO” and note issue on facility recommendations tracker.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To assess an adequate file management -- you may query if they were to look for 10 charts, how many would the find. If it is less than 10 then you have an inadequate file management system. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This indicator refers to all levels of staff, counselors, nurses etc. </t>
+  </si>
+  <si>
+    <t>To meet this indicator, all staff must reach 80% of their daily targets -- each cadre and each individual.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Does the facility have a full time facility manager? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">To calculate this indicator - the facility manager can tell you the categories of staff they have and what is vacant. </t>
+  </si>
+  <si>
+    <t>Working Definitions for Minimum Requirements Tool</t>
+  </si>
+  <si>
+    <t>Updated May 29, 2019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -645,8 +753,55 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0D0D0D"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -677,8 +832,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -746,11 +913,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -801,6 +1020,28 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1110,7 +1351,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -3025,4 +3266,168 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="60.7109375" customWidth="1"/>
+    <col min="3" max="3" width="125.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="28" t="s">
+        <v>183</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="26" t="s">
+        <v>194</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="33" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="28" t="s">
+        <v>174</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="28" t="s">
+        <v>178</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="26" t="s">
+        <v>179</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="26" t="s">
+        <v>180</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>204</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>